<commit_message>
Menu and other updates
</commit_message>
<xml_diff>
--- a/2024FEB_M1_Daily_Class.xlsx
+++ b/2024FEB_M1_Daily_Class.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
   <si>
     <t>S.N.</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>GUI Components</t>
+  </si>
+  <si>
+    <t>Menu, Menu items</t>
   </si>
 </sst>
 </file>
@@ -192,7 +195,7 @@
     <numFmt numFmtId="164" formatCode=",,"/>
     <numFmt numFmtId="165" formatCode="dddd, mmmm dd, yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +216,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -227,7 +236,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -248,6 +257,13 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -283,8 +299,8 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1433,7 +1449,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
       <c r="A76" s="10"/>
       <c r="B76" s="8">
         <v>45408</v>
@@ -1442,7 +1458,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
       <c r="A77" s="10"/>
       <c r="B77" s="8">
         <v>45409</v>
@@ -1451,7 +1467,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
       <c r="A78" s="10"/>
       <c r="B78" s="8">
         <v>45410</v>
@@ -1460,77 +1476,79 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
       <c r="A79" s="10"/>
       <c r="B79" s="8">
         <v>45411</v>
       </c>
-      <c r="C79" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
+      <c r="C79" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
       <c r="A80" s="10"/>
       <c r="B80" s="8">
         <v>45412</v>
       </c>
       <c r="C80" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5">
       <c r="A81" s="10"/>
       <c r="B81" s="8">
         <v>45413</v>
       </c>
       <c r="C81" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
       <c r="A82" s="10"/>
       <c r="B82" s="8">
         <v>45414</v>
       </c>
       <c r="C82" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
       <c r="A83" s="10"/>
       <c r="B83" s="8">
         <v>45415</v>
       </c>
       <c r="C83" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
       <c r="A84" s="10"/>
       <c r="B84" s="8">
         <v>45416</v>
       </c>
       <c r="C84" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
       <c r="A85" s="10"/>
       <c r="B85" s="8">
         <v>45417</v>
       </c>
       <c r="C85" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
       <c r="A86" s="10"/>
       <c r="B86" s="8">
         <v>45418</v>
       </c>
       <c r="C86" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
       <c r="A87" s="10"/>
       <c r="B87" s="8">
         <v>45419</v>
       </c>
       <c r="C87" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
       <c r="A88" s="10"/>
       <c r="B88" s="8">
         <v>45420</v>
       </c>
       <c r="C88" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
       <c r="A89" s="10"/>
       <c r="B89" s="8">
         <v>45421</v>

</xml_diff>